<commit_message>
Finished comparison with previous studies
</commit_message>
<xml_diff>
--- a/analysis/studies_comp.xlsx
+++ b/analysis/studies_comp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\research\papers_and_projects\2021\cop_homo_tandem_cf-vs-cg\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobua\Dropbox\research\papers_and_projects\2021\cop_homo_tandem_cf-vs-cg\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA8808EA-B704-4B66-A52E-920001AA65DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F83015B-F1DD-42E8-AC57-2B182A1EA121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{814FF396-EA8B-4D9B-B8DF-5901D2A8F417}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{814FF396-EA8B-4D9B-B8DF-5901D2A8F417}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Florida 2019</t>
   </si>
@@ -44,9 +44,6 @@
     <t>28℃</t>
   </si>
   <si>
-    <t>140mm</t>
-  </si>
-  <si>
     <t>C. gestroi</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>April 18,20</t>
   </si>
   <si>
-    <t>150mm</t>
-  </si>
-  <si>
     <t>This study</t>
   </si>
   <si>
@@ -92,26 +86,26 @@
     <t>Arena</t>
   </si>
   <si>
-    <t>Tandem events</t>
-  </si>
-  <si>
     <t>Pairs</t>
   </si>
   <si>
     <t>Ref</t>
   </si>
   <si>
-    <t>Mizumoto et al., 2021  Proc R Soc B, 288, 20210998.</t>
-  </si>
-  <si>
     <t>Mizumoto et al., 2020 J Anim Ecol, 89, 2542–2552</t>
+  </si>
+  <si>
+    <t>Tandems</t>
+  </si>
+  <si>
+    <t>Mizumoto et al., 2021  Proc R Soc B, 288, 20210998</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,37 +114,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="PT Serif"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="PT Serif"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="PT Serif"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="PT Serif"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -174,13 +177,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,173 +522,175 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
         <v>484</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
+      <c r="G2" s="3">
+        <v>140</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5">
+        <v>89</v>
+      </c>
+      <c r="E3" s="5">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>89</v>
-      </c>
-      <c r="E3" s="3">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
+      <c r="G3" s="5">
+        <v>140</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
         <v>721</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
+      <c r="G4" s="3">
+        <v>150</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>94</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
+      <c r="G5" s="3">
+        <v>140</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>421</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>49</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>12</v>
+      <c r="G6" s="1">
+        <v>150</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>